<commit_message>
containerised with a full-stack setup
</commit_message>
<xml_diff>
--- a/lead_tracker.xlsx
+++ b/lead_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,48 +456,76 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>revenue</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>match</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>email</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Food Safety and Standards Authority of India (FSSAI)</t>
+          <t>Dixon Technologies</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.fssai.gov.in/</t>
+          <t>https://dixonindia.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Regulatory body for food safety in India, responsible for ensuring food safety and hygiene standards</t>
+          <t>Dixon Technologies is an electronics manufacturing services (EMS) company</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Food inspection and testing services</t>
+          <t>LED TVs, mobile phones, home appliances</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Replicant Systems vision AI + industrial automation can help FSSAI enhance food safety by automating inspection processes</t>
+          <t>500-1000 cr</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Subject: Enhancing Food Safety with AI-Powered Inspection Solutions
-Dear FSSAI Team,
-Replicant Systems specializesizes in AI-driven vision systems and industrial automation solutions. Our technology can help automate food inspection processes.
-Best regards,
-Replicant Systems Team</t>
+          <t>Replicant Systems' vision AI can help Dixon Technologies automate inspection of LED TVs and mobile phones, reducing defects and increasing efficiency.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Optiemus Infracom</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://optiemus.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Optiemus Infracom is a telecom and electronics manufacturing company</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Telecom equipment, electronic devices, IoT solutions</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>500-1000 cr</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Replicant Systems' industrial automation solutions can assist Optiemus Infracom in streamlining telecom equipment manufacturing, improving product reliability and reducing costs.</t>
         </is>
       </c>
     </row>

</xml_diff>